<commit_message>
Object & creature class added
</commit_message>
<xml_diff>
--- a/Commits table.xlsx
+++ b/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -35,13 +35,19 @@
     <t>Commit</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
     <t>Total(h):</t>
+  </si>
+  <si>
+    <t>Commit table added</t>
+  </si>
+  <si>
+    <t>World &amp; kbhit added</t>
+  </si>
+  <si>
+    <t>Time(h)</t>
+  </si>
+  <si>
+    <t>Objects/Creatures added</t>
   </si>
 </sst>
 </file>
@@ -145,12 +151,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Énfasis5" xfId="4" builtinId="46"/>
@@ -438,7 +445,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +465,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,24 +478,36 @@
         <v>1</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="4"/>
@@ -577,11 +596,11 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="1">
         <f>SUM(E4:E24)</f>
-        <v>0</v>
+        <v>2.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>